<commit_message>
:fire: Submit new how-to iteration
</commit_message>
<xml_diff>
--- a/TESTdocs/PYJMAILER-Test_DOC.xlsx
+++ b/TESTdocs/PYJMAILER-Test_DOC.xlsx
@@ -5,23 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klych\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klych\Desktop\main\TESTdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB8EFB5-0F25-4E4A-BAD6-8F6895BB68CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC74641-19EE-4456-995A-CBEC22ACA21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -134,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t>Test case ID</t>
   </si>
@@ -214,9 +221,6 @@
     <t>On the index page</t>
   </si>
   <si>
-    <t>Check that when the user clicks the "Email" button on the captureForm page, the user is redirected to the emailingPage page</t>
-  </si>
-  <si>
     <t>Check that when the user clicks the "Home" button on the emailingPagepage, the user is redirected to the index page</t>
   </si>
   <si>
@@ -226,9 +230,6 @@
     <t>TCase_6</t>
   </si>
   <si>
-    <t>Check that when the user clicks the "Capture" button on the emailingPagepage, the user is redirected to the captureForm page</t>
-  </si>
-  <si>
     <t>klychnick512@gmail.com</t>
   </si>
   <si>
@@ -244,9 +245,6 @@
     <t>TCase_8</t>
   </si>
   <si>
-    <t>TCase_9</t>
-  </si>
-  <si>
     <t>TCase_10</t>
   </si>
   <si>
@@ -280,10 +278,7 @@
     <t>"      "</t>
   </si>
   <si>
-    <t>TCase_12</t>
-  </si>
-  <si>
-    <t>TCase_13</t>
+    <t>Tcase_9</t>
   </si>
 </sst>
 </file>
@@ -446,19 +441,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Settings"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -724,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,13 +845,13 @@
         <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="7">
         <v>44647</v>
@@ -882,21 +864,21 @@
       </c>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:10" ht="69" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F6" s="7">
         <v>44647</v>
@@ -909,21 +891,21 @@
       </c>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:10" ht="69" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="F7" s="7">
         <v>44647</v>
@@ -938,19 +920,19 @@
     </row>
     <row r="8" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8" s="7">
         <v>44647</v>
@@ -962,21 +944,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="69" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" s="7">
         <v>44647</v>
@@ -988,21 +970,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F10" s="7">
         <v>44647</v>
@@ -1014,21 +996,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="69" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>31</v>
-      </c>
       <c r="E11" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F11" s="7">
         <v>44647</v>
@@ -1042,19 +1024,19 @@
     </row>
     <row r="12" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>33</v>
+        <v>27</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F12" s="7">
         <v>44647</v>
@@ -1066,56 +1048,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="7">
-        <v>44647</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="7">
-        <v>44647</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>20</v>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <f ca="1">C5+B63</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>